<commit_message>
modified some files from laptop
</commit_message>
<xml_diff>
--- a/Bikewale Test Cases.xlsx
+++ b/Bikewale Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandesh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandesh\Desktop\Class\Projects\BikeWaleTNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1160834-47E8-4B73-919C-2B42702749CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C529C8-B411-44D0-A08C-AF22B0A7B5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="1770" windowWidth="17700" windowHeight="12645" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="4" r:id="rId1"/>
@@ -439,17 +439,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,15 +737,15 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="1"/>
-    <col min="5" max="6" width="17.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="4" width="9.109375" style="1"/>
+    <col min="5" max="6" width="17.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E8" s="5" t="s">
         <v>0</v>
       </c>
@@ -753,7 +753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
@@ -761,7 +761,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
@@ -769,7 +769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E11" s="5"/>
       <c r="F11" s="6" t="s">
         <v>23</v>
@@ -778,7 +778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E12" s="5"/>
       <c r="F12" s="6" t="s">
         <v>24</v>
@@ -787,64 +787,64 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G32" s="4"/>
     </row>
   </sheetData>
@@ -860,73 +860,73 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="70" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="41.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="41.88671875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C7" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -943,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
@@ -951,8 +951,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -972,8 +972,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="4"/>
@@ -987,154 +987,154 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1158,24 +1158,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="28.5703125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57.109375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="28.5546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1210,367 +1210,367 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9" t="s">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1582,23 +1582,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5048AE4-00C9-4E7D-A638-523FE5B24FA3}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" customWidth="1"/>
-    <col min="6" max="8" width="28.5703125" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="57.109375" customWidth="1"/>
+    <col min="6" max="8" width="28.5546875" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1633,315 +1633,315 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1955,7 +1955,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1967,7 +1967,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>